<commit_message>
Added the cities Excel
Excel with cities names
</commit_message>
<xml_diff>
--- a/inputs/cities.xlsx
+++ b/inputs/cities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SCRIPTS\immoDATA\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63BB14F3-C7E0-4A65-A850-B8674F49AD3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56F49594-B6FA-46E2-AAA9-3DE5926A6526}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="113">
   <si>
     <t>Stadt/Gemeinde</t>
   </si>
@@ -171,18 +171,12 @@
     <t>Straubing</t>
   </si>
   <si>
-    <t>Hof (Saale)</t>
-  </si>
-  <si>
     <t>Kaufbeuren</t>
   </si>
   <si>
     <t>Memmingen</t>
   </si>
   <si>
-    <t>Weiden in der Oberpfalz</t>
-  </si>
-  <si>
     <t>Oberpfalz-Nord</t>
   </si>
   <si>
@@ -255,9 +249,6 @@
     <t>Oberland</t>
   </si>
   <si>
-    <t>Lauf an der Pegnitz</t>
-  </si>
-  <si>
     <t>Nürnberger Land</t>
   </si>
   <si>
@@ -306,9 +297,6 @@
     <t>Erlangen-Höchstadt</t>
   </si>
   <si>
-    <t>Weilheim in Oberbayern</t>
-  </si>
-  <si>
     <t>Weilheim-Schongau</t>
   </si>
   <si>
@@ -366,9 +354,6 @@
     <t>Donau-Ries</t>
   </si>
   <si>
-    <t>Neufahrn bei Freising</t>
-  </si>
-  <si>
     <t>Lichtenfels</t>
   </si>
   <si>
@@ -376,6 +361,30 @@
   </si>
   <si>
     <t>Landkreis Donau-Ries</t>
+  </si>
+  <si>
+    <t>Neufahrn b. Freising</t>
+  </si>
+  <si>
+    <t>Mühldorf a. Inn</t>
+  </si>
+  <si>
+    <t>Weilheim i. OB</t>
+  </si>
+  <si>
+    <t>Pfaffenhofen a. d. Ilm</t>
+  </si>
+  <si>
+    <t>Lauf a.d. Pegnitz</t>
+  </si>
+  <si>
+    <t>Neumarkt i. d. OBp</t>
+  </si>
+  <si>
+    <t>Weiden</t>
+  </si>
+  <si>
+    <t>Hof</t>
   </si>
 </sst>
 </file>
@@ -772,7 +781,7 @@
   <dimension ref="A1:E76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1142,7 +1151,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>41</v>
+        <v>112</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>6</v>
@@ -1159,7 +1168,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>6</v>
@@ -1176,7 +1185,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>6</v>
@@ -1193,7 +1202,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>44</v>
+        <v>111</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>6</v>
@@ -1202,7 +1211,7 @@
         <v>13</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E25">
         <v>42472</v>
@@ -1210,7 +1219,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>6</v>
@@ -1219,7 +1228,7 @@
         <v>13</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E26">
         <v>41994</v>
@@ -1227,7 +1236,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>6</v>
@@ -1236,7 +1245,7 @@
         <v>9</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E27">
         <v>41662</v>
@@ -1244,7 +1253,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>6</v>
@@ -1261,7 +1270,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>6</v>
@@ -1278,10 +1287,10 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>7</v>
@@ -1295,10 +1304,10 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>53</v>
+        <v>110</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>13</v>
@@ -1312,10 +1321,10 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>7</v>
@@ -1329,10 +1338,10 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>7</v>
@@ -1346,10 +1355,10 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>25</v>
@@ -1363,10 +1372,10 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>20</v>
@@ -1380,10 +1389,10 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>11</v>
@@ -1397,10 +1406,10 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>7</v>
@@ -1414,10 +1423,10 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>7</v>
@@ -1431,7 +1440,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>5</v>
@@ -1448,16 +1457,16 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E40">
         <v>29254</v>
@@ -1465,7 +1474,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>10</v>
@@ -1482,10 +1491,10 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>7</v>
@@ -1499,16 +1508,16 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E43">
         <v>27249</v>
@@ -1516,10 +1525,10 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>69</v>
+        <v>109</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>9</v>
@@ -1533,10 +1542,10 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>71</v>
+        <v>108</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>7</v>
@@ -1550,10 +1559,10 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>20</v>
@@ -1567,7 +1576,7 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>15</v>
@@ -1584,10 +1593,10 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>9</v>
@@ -1601,10 +1610,10 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>11</v>
@@ -1618,16 +1627,16 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E50">
         <v>25221</v>
@@ -1635,7 +1644,7 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>5</v>
@@ -1652,10 +1661,10 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>7</v>
@@ -1669,10 +1678,10 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>7</v>
@@ -1686,10 +1695,10 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>7</v>
@@ -1703,10 +1712,10 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>9</v>
@@ -1720,16 +1729,16 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>86</v>
+        <v>107</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E56">
         <v>22703</v>
@@ -1737,7 +1746,7 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>10</v>
@@ -1754,10 +1763,10 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>17</v>
@@ -1771,7 +1780,7 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>32</v>
@@ -1788,7 +1797,7 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>10</v>
@@ -1805,10 +1814,10 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>17</v>
@@ -1822,7 +1831,7 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>39</v>
@@ -1839,7 +1848,7 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>5</v>
@@ -1856,10 +1865,10 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>11</v>
@@ -1873,10 +1882,10 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>7</v>
@@ -1890,10 +1899,10 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>11</v>
@@ -1907,7 +1916,7 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>5</v>
@@ -1924,10 +1933,10 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>7</v>
@@ -1941,10 +1950,10 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>11</v>
@@ -1958,10 +1967,10 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>7</v>
@@ -1975,10 +1984,10 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>7</v>
@@ -1992,10 +2001,10 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>11</v>
@@ -2009,10 +2018,10 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>81</v>
+        <v>106</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>7</v>
@@ -2026,7 +2035,7 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>38</v>
@@ -2043,10 +2052,10 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>20</v>
@@ -2060,10 +2069,10 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
gitignore + Distance Added, Filter Anwenden
Distance Option Added, Filter Anwenden
</commit_message>
<xml_diff>
--- a/inputs/cities.xlsx
+++ b/inputs/cities.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SCRIPTS\immoDATA\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56F49594-B6FA-46E2-AAA9-3DE5926A6526}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0F17ACB-F91D-49E2-BA84-35C838CDA68A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bayern" sheetId="2" r:id="rId1"/>
+    <sheet name="Munich_Area" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="ExternalData_1" localSheetId="0" hidden="1">Bayern!$A$1:$E$76</definedName>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="113">
   <si>
     <t>Stadt/Gemeinde</t>
   </si>
@@ -420,9 +421,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -780,8 +780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="A74" activeCellId="1" sqref="A70:XFD70 A74:XFD74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -810,16 +810,16 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
         <v>5</v>
       </c>
       <c r="E2">
@@ -827,16 +827,16 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" t="s">
         <v>8</v>
       </c>
       <c r="E3">
@@ -844,16 +844,16 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" t="s">
         <v>10</v>
       </c>
       <c r="E4">
@@ -861,16 +861,16 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="1" t="s">
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" t="s">
         <v>12</v>
       </c>
       <c r="E5">
@@ -878,16 +878,16 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="1" t="s">
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
         <v>14</v>
       </c>
       <c r="E6">
@@ -895,16 +895,16 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="1" t="s">
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" t="s">
         <v>8</v>
       </c>
       <c r="E7">
@@ -912,16 +912,16 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="1" t="s">
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" t="s">
         <v>16</v>
       </c>
       <c r="E8">
@@ -929,16 +929,16 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="1" t="s">
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" t="s">
         <v>8</v>
       </c>
       <c r="E9">
@@ -946,16 +946,16 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="1" t="s">
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" t="s">
         <v>21</v>
       </c>
       <c r="E10">
@@ -963,16 +963,16 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="1" t="s">
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" t="s">
         <v>23</v>
       </c>
       <c r="E11">
@@ -980,16 +980,16 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="A12" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="1" t="s">
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" t="s">
         <v>24</v>
       </c>
       <c r="E12">
@@ -997,16 +997,16 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="A13" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="1" t="s">
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" t="s">
         <v>27</v>
       </c>
       <c r="E13">
@@ -1014,16 +1014,16 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="A14" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" s="1" t="s">
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" t="s">
         <v>29</v>
       </c>
       <c r="E14">
@@ -1031,16 +1031,16 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="A15" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" s="1" t="s">
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" t="s">
         <v>31</v>
       </c>
       <c r="E15">
@@ -1048,16 +1048,16 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="A16" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" t="s">
         <v>33</v>
       </c>
       <c r="E16">
@@ -1065,16 +1065,16 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="A17" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" s="1" t="s">
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" t="s">
         <v>35</v>
       </c>
       <c r="E17">
@@ -1082,16 +1082,16 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="A18" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" s="1" t="s">
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" t="s">
         <v>37</v>
       </c>
       <c r="E18">
@@ -1099,16 +1099,16 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="A19" t="s">
         <v>38</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D19" s="1" t="s">
+      <c r="C19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" t="s">
         <v>5</v>
       </c>
       <c r="E19">
@@ -1116,16 +1116,16 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="A20" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" t="s">
         <v>39</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D20" s="1" t="s">
+      <c r="C20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" t="s">
         <v>5</v>
       </c>
       <c r="E20">
@@ -1133,16 +1133,16 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="A21" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" s="1" t="s">
+      <c r="B21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" t="s">
         <v>25</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D21" t="s">
         <v>37</v>
       </c>
       <c r="E21">
@@ -1150,16 +1150,16 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="A22" t="s">
         <v>112</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C22" s="1" t="s">
+      <c r="B22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" t="s">
         <v>20</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D22" t="s">
         <v>23</v>
       </c>
       <c r="E22">
@@ -1167,16 +1167,16 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+      <c r="A23" t="s">
         <v>41</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C23" s="1" t="s">
+      <c r="B23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" t="s">
         <v>11</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D23" t="s">
         <v>29</v>
       </c>
       <c r="E23">
@@ -1184,16 +1184,16 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="A24" t="s">
         <v>42</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C24" s="1" t="s">
+      <c r="B24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" t="s">
         <v>11</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D24" t="s">
         <v>33</v>
       </c>
       <c r="E24">
@@ -1201,16 +1201,16 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+      <c r="A25" t="s">
         <v>111</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C25" s="1" t="s">
+      <c r="B25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" t="s">
         <v>13</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D25" t="s">
         <v>43</v>
       </c>
       <c r="E25">
@@ -1218,16 +1218,16 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+      <c r="A26" t="s">
         <v>44</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C26" s="1" t="s">
+      <c r="B26" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" t="s">
         <v>13</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D26" t="s">
         <v>43</v>
       </c>
       <c r="E26">
@@ -1235,16 +1235,16 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+      <c r="A27" t="s">
         <v>45</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C27" s="1" t="s">
+      <c r="B27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" t="s">
         <v>9</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D27" t="s">
         <v>46</v>
       </c>
       <c r="E27">
@@ -1252,16 +1252,16 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+      <c r="A28" t="s">
         <v>47</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C28" s="1" t="s">
+      <c r="B28" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" t="s">
         <v>20</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D28" t="s">
         <v>21</v>
       </c>
       <c r="E28">
@@ -1269,16 +1269,16 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+      <c r="A29" t="s">
         <v>48</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C29" s="1" t="s">
+      <c r="B29" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" t="s">
         <v>9</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="D29" t="s">
         <v>8</v>
       </c>
       <c r="E29">
@@ -1286,16 +1286,16 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+      <c r="A30" t="s">
         <v>49</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" t="s">
         <v>50</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D30" s="1" t="s">
+      <c r="C30" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" t="s">
         <v>5</v>
       </c>
       <c r="E30">
@@ -1303,16 +1303,16 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+      <c r="A31" t="s">
         <v>110</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" t="s">
         <v>51</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" t="s">
         <v>13</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D31" t="s">
         <v>12</v>
       </c>
       <c r="E31">
@@ -1320,16 +1320,16 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+      <c r="A32" t="s">
         <v>50</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" t="s">
         <v>50</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D32" s="1" t="s">
+      <c r="C32" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" t="s">
         <v>5</v>
       </c>
       <c r="E32">
@@ -1337,16 +1337,16 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+      <c r="A33" t="s">
         <v>52</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" t="s">
         <v>52</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D33" s="1" t="s">
+      <c r="C33" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" t="s">
         <v>5</v>
       </c>
       <c r="E33">
@@ -1354,16 +1354,16 @@
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+      <c r="A34" t="s">
         <v>53</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" t="s">
         <v>53</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C34" t="s">
         <v>25</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D34" t="s">
         <v>37</v>
       </c>
       <c r="E34">
@@ -1371,16 +1371,16 @@
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+      <c r="A35" t="s">
         <v>54</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" t="s">
         <v>55</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C35" t="s">
         <v>20</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D35" t="s">
         <v>21</v>
       </c>
       <c r="E35">
@@ -1388,16 +1388,16 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+      <c r="A36" t="s">
         <v>56</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B36" t="s">
         <v>57</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C36" t="s">
         <v>11</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D36" t="s">
         <v>10</v>
       </c>
       <c r="E36">
@@ -1405,16 +1405,16 @@
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
+      <c r="A37" t="s">
         <v>58</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B37" t="s">
         <v>59</v>
       </c>
-      <c r="C37" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D37" s="1" t="s">
+      <c r="C37" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" t="s">
         <v>14</v>
       </c>
       <c r="E37">
@@ -1422,16 +1422,16 @@
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
+      <c r="A38" t="s">
         <v>60</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B38" t="s">
         <v>60</v>
       </c>
-      <c r="C38" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D38" s="1" t="s">
+      <c r="C38" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38" t="s">
         <v>5</v>
       </c>
       <c r="E38">
@@ -1439,16 +1439,16 @@
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
+      <c r="A39" t="s">
         <v>61</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D39" s="1" t="s">
+      <c r="B39" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39" t="s">
+        <v>7</v>
+      </c>
+      <c r="D39" t="s">
         <v>5</v>
       </c>
       <c r="E39">
@@ -1456,16 +1456,16 @@
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
+      <c r="A40" t="s">
         <v>62</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" t="s">
         <v>62</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C40" t="s">
         <v>13</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="D40" t="s">
         <v>43</v>
       </c>
       <c r="E40">
@@ -1473,16 +1473,16 @@
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
+      <c r="A41" t="s">
         <v>63</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B41" t="s">
         <v>10</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C41" t="s">
         <v>11</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="D41" t="s">
         <v>10</v>
       </c>
       <c r="E41">
@@ -1490,16 +1490,16 @@
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
+      <c r="A42" t="s">
         <v>64</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B42" t="s">
         <v>50</v>
       </c>
-      <c r="C42" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D42" s="1" t="s">
+      <c r="C42" t="s">
+        <v>7</v>
+      </c>
+      <c r="D42" t="s">
         <v>5</v>
       </c>
       <c r="E42">
@@ -1507,16 +1507,16 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
+      <c r="A43" t="s">
         <v>65</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B43" t="s">
         <v>65</v>
       </c>
-      <c r="C43" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D43" s="1" t="s">
+      <c r="C43" t="s">
+        <v>7</v>
+      </c>
+      <c r="D43" t="s">
         <v>66</v>
       </c>
       <c r="E43">
@@ -1524,16 +1524,16 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
+      <c r="A44" t="s">
         <v>109</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B44" t="s">
         <v>67</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="C44" t="s">
         <v>9</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="D44" t="s">
         <v>8</v>
       </c>
       <c r="E44">
@@ -1541,16 +1541,16 @@
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
+      <c r="A45" t="s">
         <v>108</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B45" t="s">
         <v>68</v>
       </c>
-      <c r="C45" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D45" s="1" t="s">
+      <c r="C45" t="s">
+        <v>7</v>
+      </c>
+      <c r="D45" t="s">
         <v>14</v>
       </c>
       <c r="E45">
@@ -1558,16 +1558,16 @@
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
+      <c r="A46" t="s">
         <v>69</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B46" t="s">
         <v>69</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C46" t="s">
         <v>20</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="D46" t="s">
         <v>23</v>
       </c>
       <c r="E46">
@@ -1575,16 +1575,16 @@
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
+      <c r="A47" t="s">
         <v>70</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B47" t="s">
         <v>15</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="C47" t="s">
         <v>9</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="D47" t="s">
         <v>8</v>
       </c>
       <c r="E47">
@@ -1592,16 +1592,16 @@
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
+      <c r="A48" t="s">
         <v>71</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B48" t="s">
         <v>71</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C48" t="s">
         <v>9</v>
       </c>
-      <c r="D48" s="1" t="s">
+      <c r="D48" t="s">
         <v>8</v>
       </c>
       <c r="E48">
@@ -1609,16 +1609,16 @@
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
+      <c r="A49" t="s">
         <v>72</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B49" t="s">
         <v>72</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C49" t="s">
         <v>11</v>
       </c>
-      <c r="D49" s="1" t="s">
+      <c r="D49" t="s">
         <v>29</v>
       </c>
       <c r="E49">
@@ -1626,16 +1626,16 @@
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
+      <c r="A50" t="s">
         <v>73</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B50" t="s">
         <v>74</v>
       </c>
-      <c r="C50" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D50" s="1" t="s">
+      <c r="C50" t="s">
+        <v>7</v>
+      </c>
+      <c r="D50" t="s">
         <v>66</v>
       </c>
       <c r="E50">
@@ -1643,16 +1643,16 @@
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
+      <c r="A51" t="s">
         <v>75</v>
       </c>
-      <c r="B51" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D51" s="1" t="s">
+      <c r="B51" t="s">
+        <v>5</v>
+      </c>
+      <c r="C51" t="s">
+        <v>7</v>
+      </c>
+      <c r="D51" t="s">
         <v>5</v>
       </c>
       <c r="E51">
@@ -1660,16 +1660,16 @@
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
+      <c r="A52" t="s">
         <v>76</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B52" t="s">
         <v>76</v>
       </c>
-      <c r="C52" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D52" s="1" t="s">
+      <c r="C52" t="s">
+        <v>7</v>
+      </c>
+      <c r="D52" t="s">
         <v>5</v>
       </c>
       <c r="E52">
@@ -1677,16 +1677,16 @@
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
+      <c r="A53" t="s">
         <v>77</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="B53" t="s">
         <v>78</v>
       </c>
-      <c r="C53" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D53" s="1" t="s">
+      <c r="C53" t="s">
+        <v>7</v>
+      </c>
+      <c r="D53" t="s">
         <v>31</v>
       </c>
       <c r="E53">
@@ -1694,16 +1694,16 @@
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
+      <c r="A54" t="s">
         <v>79</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="B54" t="s">
         <v>80</v>
       </c>
-      <c r="C54" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D54" s="1" t="s">
+      <c r="C54" t="s">
+        <v>7</v>
+      </c>
+      <c r="D54" t="s">
         <v>5</v>
       </c>
       <c r="E54">
@@ -1711,16 +1711,16 @@
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
+      <c r="A55" t="s">
         <v>81</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B55" t="s">
         <v>82</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="C55" t="s">
         <v>9</v>
       </c>
-      <c r="D55" s="1" t="s">
+      <c r="D55" t="s">
         <v>8</v>
       </c>
       <c r="E55">
@@ -1728,16 +1728,16 @@
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
+      <c r="A56" t="s">
         <v>107</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B56" t="s">
         <v>83</v>
       </c>
-      <c r="C56" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D56" s="1" t="s">
+      <c r="C56" t="s">
+        <v>7</v>
+      </c>
+      <c r="D56" t="s">
         <v>66</v>
       </c>
       <c r="E56">
@@ -1745,16 +1745,16 @@
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
+      <c r="A57" t="s">
         <v>84</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B57" t="s">
         <v>10</v>
       </c>
-      <c r="C57" s="1" t="s">
+      <c r="C57" t="s">
         <v>11</v>
       </c>
-      <c r="D57" s="1" t="s">
+      <c r="D57" t="s">
         <v>10</v>
       </c>
       <c r="E57">
@@ -1762,16 +1762,16 @@
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
+      <c r="A58" t="s">
         <v>85</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B58" t="s">
         <v>85</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="C58" t="s">
         <v>17</v>
       </c>
-      <c r="D58" s="1" t="s">
+      <c r="D58" t="s">
         <v>35</v>
       </c>
       <c r="E58">
@@ -1779,16 +1779,16 @@
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
+      <c r="A59" t="s">
         <v>86</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B59" t="s">
         <v>32</v>
       </c>
-      <c r="C59" s="1" t="s">
+      <c r="C59" t="s">
         <v>11</v>
       </c>
-      <c r="D59" s="1" t="s">
+      <c r="D59" t="s">
         <v>33</v>
       </c>
       <c r="E59">
@@ -1796,16 +1796,16 @@
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
+      <c r="A60" t="s">
         <v>87</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B60" t="s">
         <v>10</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="C60" t="s">
         <v>11</v>
       </c>
-      <c r="D60" s="1" t="s">
+      <c r="D60" t="s">
         <v>10</v>
       </c>
       <c r="E60">
@@ -1813,16 +1813,16 @@
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
+      <c r="A61" t="s">
         <v>88</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B61" t="s">
         <v>88</v>
       </c>
-      <c r="C61" s="1" t="s">
+      <c r="C61" t="s">
         <v>17</v>
       </c>
-      <c r="D61" s="1" t="s">
+      <c r="D61" t="s">
         <v>16</v>
       </c>
       <c r="E61">
@@ -1830,16 +1830,16 @@
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
+      <c r="A62" t="s">
         <v>89</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="B62" t="s">
         <v>39</v>
       </c>
-      <c r="C62" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D62" s="1" t="s">
+      <c r="C62" t="s">
+        <v>7</v>
+      </c>
+      <c r="D62" t="s">
         <v>5</v>
       </c>
       <c r="E62">
@@ -1847,16 +1847,16 @@
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
+      <c r="A63" t="s">
         <v>90</v>
       </c>
-      <c r="B63" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D63" s="1" t="s">
+      <c r="B63" t="s">
+        <v>5</v>
+      </c>
+      <c r="C63" t="s">
+        <v>7</v>
+      </c>
+      <c r="D63" t="s">
         <v>5</v>
       </c>
       <c r="E63">
@@ -1864,16 +1864,16 @@
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
+      <c r="A64" t="s">
         <v>91</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="B64" t="s">
         <v>92</v>
       </c>
-      <c r="C64" s="1" t="s">
+      <c r="C64" t="s">
         <v>11</v>
       </c>
-      <c r="D64" s="1" t="s">
+      <c r="D64" t="s">
         <v>29</v>
       </c>
       <c r="E64">
@@ -1881,16 +1881,16 @@
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
+      <c r="A65" t="s">
         <v>93</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="B65" t="s">
         <v>50</v>
       </c>
-      <c r="C65" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D65" s="1" t="s">
+      <c r="C65" t="s">
+        <v>7</v>
+      </c>
+      <c r="D65" t="s">
         <v>5</v>
       </c>
       <c r="E65">
@@ -1898,16 +1898,16 @@
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
+      <c r="A66" t="s">
         <v>94</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="B66" t="s">
         <v>57</v>
       </c>
-      <c r="C66" s="1" t="s">
+      <c r="C66" t="s">
         <v>11</v>
       </c>
-      <c r="D66" s="1" t="s">
+      <c r="D66" t="s">
         <v>10</v>
       </c>
       <c r="E66">
@@ -1915,16 +1915,16 @@
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
+      <c r="A67" t="s">
         <v>95</v>
       </c>
-      <c r="B67" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D67" s="1" t="s">
+      <c r="B67" t="s">
+        <v>5</v>
+      </c>
+      <c r="C67" t="s">
+        <v>7</v>
+      </c>
+      <c r="D67" t="s">
         <v>5</v>
       </c>
       <c r="E67">
@@ -1932,16 +1932,16 @@
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
+      <c r="A68" t="s">
         <v>96</v>
       </c>
-      <c r="B68" s="1" t="s">
+      <c r="B68" t="s">
         <v>97</v>
       </c>
-      <c r="C68" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D68" s="1" t="s">
+      <c r="C68" t="s">
+        <v>7</v>
+      </c>
+      <c r="D68" t="s">
         <v>31</v>
       </c>
       <c r="E68">
@@ -1949,16 +1949,16 @@
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
+      <c r="A69" t="s">
         <v>98</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="B69" t="s">
         <v>98</v>
       </c>
-      <c r="C69" s="1" t="s">
+      <c r="C69" t="s">
         <v>11</v>
       </c>
-      <c r="D69" s="1" t="s">
+      <c r="D69" t="s">
         <v>33</v>
       </c>
       <c r="E69">
@@ -1966,16 +1966,16 @@
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
+      <c r="A70" t="s">
         <v>99</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="B70" t="s">
         <v>76</v>
       </c>
-      <c r="C70" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D70" s="1" t="s">
+      <c r="C70" t="s">
+        <v>7</v>
+      </c>
+      <c r="D70" t="s">
         <v>5</v>
       </c>
       <c r="E70">
@@ -1983,16 +1983,16 @@
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="1" t="s">
+      <c r="A71" t="s">
         <v>97</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="B71" t="s">
         <v>97</v>
       </c>
-      <c r="C71" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D71" s="1" t="s">
+      <c r="C71" t="s">
+        <v>7</v>
+      </c>
+      <c r="D71" t="s">
         <v>31</v>
       </c>
       <c r="E71">
@@ -2000,16 +2000,16 @@
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="1" t="s">
+      <c r="A72" t="s">
         <v>100</v>
       </c>
-      <c r="B72" s="1" t="s">
+      <c r="B72" t="s">
         <v>101</v>
       </c>
-      <c r="C72" s="1" t="s">
+      <c r="C72" t="s">
         <v>11</v>
       </c>
-      <c r="D72" s="1" t="s">
+      <c r="D72" t="s">
         <v>10</v>
       </c>
       <c r="E72">
@@ -2017,16 +2017,16 @@
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="1" t="s">
+      <c r="A73" t="s">
         <v>106</v>
       </c>
-      <c r="B73" s="1" t="s">
+      <c r="B73" t="s">
         <v>78</v>
       </c>
-      <c r="C73" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D73" s="1" t="s">
+      <c r="C73" t="s">
+        <v>7</v>
+      </c>
+      <c r="D73" t="s">
         <v>31</v>
       </c>
       <c r="E73">
@@ -2034,16 +2034,16 @@
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="1" t="s">
+      <c r="A74" t="s">
         <v>105</v>
       </c>
-      <c r="B74" s="1" t="s">
+      <c r="B74" t="s">
         <v>38</v>
       </c>
-      <c r="C74" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D74" s="1" t="s">
+      <c r="C74" t="s">
+        <v>7</v>
+      </c>
+      <c r="D74" t="s">
         <v>5</v>
       </c>
       <c r="E74">
@@ -2051,16 +2051,16 @@
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
+      <c r="A75" t="s">
         <v>102</v>
       </c>
-      <c r="B75" s="1" t="s">
+      <c r="B75" t="s">
         <v>102</v>
       </c>
-      <c r="C75" s="1" t="s">
+      <c r="C75" t="s">
         <v>20</v>
       </c>
-      <c r="D75" s="1" t="s">
+      <c r="D75" t="s">
         <v>21</v>
       </c>
       <c r="E75">
@@ -2068,16 +2068,16 @@
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="1" t="s">
+      <c r="A76" t="s">
         <v>103</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="B76" t="s">
         <v>104</v>
       </c>
-      <c r="C76" s="1" t="s">
+      <c r="C76" t="s">
         <v>11</v>
       </c>
-      <c r="D76" s="1" t="s">
+      <c r="D76" t="s">
         <v>10</v>
       </c>
       <c r="E76">
@@ -2089,6 +2089,436 @@
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC5365BF-56CB-45AB-91BC-4BEE9B15F190}">
+  <dimension ref="A1:E24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <v>1487708</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3">
+        <v>510632</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4">
+        <v>296478</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5">
+        <v>153542</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6">
+        <v>138016</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7">
+        <v>73150</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8">
+        <v>63508</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9">
+        <v>48582</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10">
+        <v>47738</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11">
+        <v>37063</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12">
+        <v>36414</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13">
+        <v>29344</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14">
+        <v>28896</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15">
+        <v>27653</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>75</v>
+      </c>
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16">
+        <v>25379</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>76</v>
+      </c>
+      <c r="B17" t="s">
+        <v>76</v>
+      </c>
+      <c r="C17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17">
+        <v>23453</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>79</v>
+      </c>
+      <c r="B18" t="s">
+        <v>80</v>
+      </c>
+      <c r="C18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18">
+        <v>25023</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>89</v>
+      </c>
+      <c r="B19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19">
+        <v>21853</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>90</v>
+      </c>
+      <c r="B20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20">
+        <v>21719</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>93</v>
+      </c>
+      <c r="B21" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21">
+        <v>21221</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>95</v>
+      </c>
+      <c r="B22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22">
+        <v>21797</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>99</v>
+      </c>
+      <c r="B23" t="s">
+        <v>76</v>
+      </c>
+      <c r="C23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" t="s">
+        <v>5</v>
+      </c>
+      <c r="E23">
+        <v>20829</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>105</v>
+      </c>
+      <c r="B24" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" t="s">
+        <v>5</v>
+      </c>
+      <c r="E24">
+        <v>20202</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>